<commit_message>
created pickle files for the dataframes and the dictionaries
</commit_message>
<xml_diff>
--- a/Documents/Soccer/manager.xlsx
+++ b/Documents/Soccer/manager.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12760" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="129">
   <si>
     <t>Hull City FC</t>
   </si>
@@ -329,26 +329,109 @@
     <t>nationality</t>
   </si>
   <si>
-    <t>Marco Saravia</t>
-  </si>
-  <si>
     <t>1977-07-12</t>
   </si>
   <si>
     <t>Portugal</t>
+  </si>
+  <si>
+    <t>Marco Silva</t>
+  </si>
+  <si>
+    <t>Criag Shakespeare</t>
+  </si>
+  <si>
+    <t>1963-10-26</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Claude Puel</t>
+  </si>
+  <si>
+    <t>1961-09-02</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Walter Mazzarri</t>
+  </si>
+  <si>
+    <t>1961-10-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italy </t>
+  </si>
+  <si>
+    <t>Steve Agnew</t>
+  </si>
+  <si>
+    <t>1965-11-09</t>
+  </si>
+  <si>
+    <t>Mark Hughes</t>
+  </si>
+  <si>
+    <t>1963-11-01</t>
+  </si>
+  <si>
+    <t>Wales</t>
+  </si>
+  <si>
+    <t>Ronald Koeman</t>
+  </si>
+  <si>
+    <t>1963-03-21</t>
+  </si>
+  <si>
+    <t>Neatherlands</t>
+  </si>
+  <si>
+    <t>Mauricio Pochettino</t>
+  </si>
+  <si>
+    <t>1972-03-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argentina </t>
+  </si>
+  <si>
+    <t>Sam Allardyce</t>
+  </si>
+  <si>
+    <t>1954-10-19</t>
+  </si>
+  <si>
+    <t>Tony Pulis</t>
+  </si>
+  <si>
+    <t>1958-01-16</t>
+  </si>
+  <si>
+    <t>Sean Dyche</t>
+  </si>
+  <si>
+    <t>1971-06-28</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -371,9 +454,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,14 +738,15 @@
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -680,66 +765,156 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
         <v>101</v>
       </c>
-      <c r="D2" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
       <c r="B3" t="s">
         <v>76</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>114</v>
+      </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>117</v>
+      </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>125</v>
+      </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
       <c r="B12" t="s">
         <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added more managers to teh manager csv file
</commit_message>
<xml_diff>
--- a/Documents/Soccer/manager.xlsx
+++ b/Documents/Soccer/manager.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="184">
   <si>
     <t>Hull City FC</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Bologna FC</t>
   </si>
   <si>
-    <t>33	FC Crotone</t>
-  </si>
-  <si>
     <t>US CittÌÁ di Palermo</t>
   </si>
   <si>
@@ -414,13 +411,181 @@
   </si>
   <si>
     <t>1971-06-28</t>
+  </si>
+  <si>
+    <t>Paul Clement</t>
+  </si>
+  <si>
+    <t>1972-01-08</t>
+  </si>
+  <si>
+    <t>Josep Guardiola</t>
+  </si>
+  <si>
+    <t>1971-01-18</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>David William Moyes</t>
+  </si>
+  <si>
+    <t>1963-04-25</t>
+  </si>
+  <si>
+    <t>Scotland</t>
+  </si>
+  <si>
+    <t>Edward Howe</t>
+  </si>
+  <si>
+    <t>1977-11-29</t>
+  </si>
+  <si>
+    <t>José Mourinho</t>
+  </si>
+  <si>
+    <t>1963-01-26</t>
+  </si>
+  <si>
+    <t>Arsène Wenger</t>
+  </si>
+  <si>
+    <t>1949-10-22</t>
+  </si>
+  <si>
+    <t>Jürgen Klopp</t>
+  </si>
+  <si>
+    <t>1967-06-16</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Antonio Conte</t>
+  </si>
+  <si>
+    <t>1969-07-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">italy </t>
+  </si>
+  <si>
+    <t>Slaven Bilić</t>
+  </si>
+  <si>
+    <t>1968-09-11</t>
+  </si>
+  <si>
+    <t>Yugoslavia</t>
+  </si>
+  <si>
+    <t>Luciano Spalletti</t>
+  </si>
+  <si>
+    <t>1959-03-07</t>
+  </si>
+  <si>
+    <t>Luigi Delneri</t>
+  </si>
+  <si>
+    <t>1950-08-23</t>
+  </si>
+  <si>
+    <t>Massimiliano Allegri</t>
+  </si>
+  <si>
+    <t>1967-08-11</t>
+  </si>
+  <si>
+    <t>Paulo Sousa</t>
+  </si>
+  <si>
+    <t>1970-08-30</t>
+  </si>
+  <si>
+    <t>Vincenzo Montella</t>
+  </si>
+  <si>
+    <t>1974-06-18</t>
+  </si>
+  <si>
+    <t>Siniša Mihajlović</t>
+  </si>
+  <si>
+    <t>1969-02-20</t>
+  </si>
+  <si>
+    <t>Rolando Maran</t>
+  </si>
+  <si>
+    <t>1963-07-14</t>
+  </si>
+  <si>
+    <t>Stefano Pioli</t>
+  </si>
+  <si>
+    <t>1965-10-20</t>
+  </si>
+  <si>
+    <t>Giovanni Martusciello</t>
+  </si>
+  <si>
+    <t>1971-08-19</t>
+  </si>
+  <si>
+    <t>Marco Giampaolo</t>
+  </si>
+  <si>
+    <t>1967-08-02</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Andrea Mandorlini</t>
+  </si>
+  <si>
+    <t>1960-07-17</t>
+  </si>
+  <si>
+    <t>Massimo Rastelli</t>
+  </si>
+  <si>
+    <t>1968-12-27</t>
+  </si>
+  <si>
+    <t>Roberto Donadoni</t>
+  </si>
+  <si>
+    <t>1963-09-09</t>
+  </si>
+  <si>
+    <t>FC Crotone</t>
+  </si>
+  <si>
+    <t>Davide Nicola</t>
+  </si>
+  <si>
+    <t>1973-03-05</t>
+  </si>
+  <si>
+    <t>Diego López</t>
+  </si>
+  <si>
+    <t>1974-08-22</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -432,6 +597,11 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -454,10 +624,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,13 +908,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
@@ -751,595 +922,811 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
         <v>96</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" t="s">
         <v>98</v>
-      </c>
-      <c r="D1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" t="s">
         <v>100</v>
-      </c>
-      <c r="D2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
         <v>104</v>
-      </c>
-      <c r="D3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" t="s">
         <v>107</v>
-      </c>
-      <c r="D4" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" t="s">
         <v>110</v>
-      </c>
-      <c r="D5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" t="s">
         <v>115</v>
-      </c>
-      <c r="D7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" t="s">
         <v>118</v>
-      </c>
-      <c r="D8" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
         <v>121</v>
-      </c>
-      <c r="D9" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>128</v>
       </c>
-      <c r="D12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>10</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>130</v>
+      </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>133</v>
+      </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>136</v>
+      </c>
       <c r="B16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>138</v>
+      </c>
       <c r="B17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>140</v>
+      </c>
       <c r="B18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>142</v>
+      </c>
       <c r="B19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>145</v>
+      </c>
       <c r="B20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>148</v>
+      </c>
       <c r="B21" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C21" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="B22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>153</v>
+      </c>
       <c r="B23" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C23" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>155</v>
+      </c>
       <c r="B24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C24" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>157</v>
+      </c>
       <c r="B25" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>159</v>
+      </c>
       <c r="B26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C26" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>161</v>
+      </c>
       <c r="B27" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C27" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D27" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>163</v>
+      </c>
       <c r="B28" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C28" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>165</v>
+      </c>
       <c r="B29" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C29" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>167</v>
+      </c>
       <c r="B30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C30" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>169</v>
+      </c>
       <c r="B31" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C31" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>172</v>
+      </c>
       <c r="B32" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C32" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>174</v>
+      </c>
       <c r="B33" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C33" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>176</v>
+      </c>
       <c r="B34" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C34" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>179</v>
+      </c>
       <c r="B35" t="s">
+        <v>178</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>181</v>
+      </c>
+      <c r="B36" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
+      <c r="C36" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D36" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed the managers csv file
</commit_message>
<xml_diff>
--- a/Documents/Soccer/manager.xlsx
+++ b/Documents/Soccer/manager.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="318">
   <si>
     <t>Hull City FC</t>
   </si>
@@ -143,9 +143,6 @@
     <t>SS Lazio</t>
   </si>
   <si>
-    <t>MÌÁlaga CF</t>
-  </si>
-  <si>
     <t>CA Osasuna</t>
   </si>
   <si>
@@ -173,24 +170,12 @@
     <t>RCD Espanyol</t>
   </si>
   <si>
-    <t>Sporting GijÌ_n</t>
-  </si>
-  <si>
     <t>Athletic Club</t>
   </si>
   <si>
-    <t>Real Sociedad de FÌ¼tbol</t>
-  </si>
-  <si>
     <t>Real Madrid CF</t>
   </si>
   <si>
-    <t>Club AtlÌ©tico de Madrid</t>
-  </si>
-  <si>
-    <t>Deportivo AlavÌ©s</t>
-  </si>
-  <si>
     <t>RC Celta de Vigo</t>
   </si>
   <si>
@@ -209,9 +194,6 @@
     <t>Ludogorez Rasgrad</t>
   </si>
   <si>
-    <t>FC Bayern MÌ_nchen</t>
-  </si>
-  <si>
     <t>FC Rostov</t>
   </si>
   <si>
@@ -266,9 +248,6 @@
     <t>CSKA Moscow</t>
   </si>
   <si>
-    <t>Bor. MÌ¦nchengladbach</t>
-  </si>
-  <si>
     <t>AS Monaco FC</t>
   </si>
   <si>
@@ -296,9 +275,6 @@
     <t>FC Ingolstadt 04</t>
   </si>
   <si>
-    <t>1. FC KÌ¦ln</t>
-  </si>
-  <si>
     <t xml:space="preserve">	SV Darmstadt 98</t>
   </si>
   <si>
@@ -383,9 +359,6 @@
     <t>1963-03-21</t>
   </si>
   <si>
-    <t>Neatherlands</t>
-  </si>
-  <si>
     <t>Mauricio Pochettino</t>
   </si>
   <si>
@@ -579,6 +552,435 @@
   </si>
   <si>
     <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Eusebio Di Francesco</t>
+  </si>
+  <si>
+    <t>1969-09-08</t>
+  </si>
+  <si>
+    <t>Zdeněk Zeman</t>
+  </si>
+  <si>
+    <t>1947-05-12</t>
+  </si>
+  <si>
+    <t>Czechoslovakia</t>
+  </si>
+  <si>
+    <t>Maurizio Sarri</t>
+  </si>
+  <si>
+    <t>1959-01-10</t>
+  </si>
+  <si>
+    <t>Gian Piero Gasperini</t>
+  </si>
+  <si>
+    <t>1958-01-26</t>
+  </si>
+  <si>
+    <t>Simone Inzaghi</t>
+  </si>
+  <si>
+    <t>1976-04-05</t>
+  </si>
+  <si>
+    <t>Míchel</t>
+  </si>
+  <si>
+    <t>Málaga CF</t>
+  </si>
+  <si>
+    <t>1963-03-23</t>
+  </si>
+  <si>
+    <t>Petar Vasiljević</t>
+  </si>
+  <si>
+    <t>1970-11-03</t>
+  </si>
+  <si>
+    <t>Pepe Mel</t>
+  </si>
+  <si>
+    <t>1963-02-28</t>
+  </si>
+  <si>
+    <t>José Luis Mendilibar</t>
+  </si>
+  <si>
+    <t>1961-03-14</t>
+  </si>
+  <si>
+    <t>Luis Enrique</t>
+  </si>
+  <si>
+    <t>1970-05-08</t>
+  </si>
+  <si>
+    <t>Víctor Sánchez</t>
+  </si>
+  <si>
+    <t>1976-02-23</t>
+  </si>
+  <si>
+    <t>Lucas Alcaraz</t>
+  </si>
+  <si>
+    <t>1966-06-21</t>
+  </si>
+  <si>
+    <t>Fran Escribá</t>
+  </si>
+  <si>
+    <t>1965-05-03</t>
+  </si>
+  <si>
+    <t>Jorge Sampaoli</t>
+  </si>
+  <si>
+    <t>1960-03-13</t>
+  </si>
+  <si>
+    <t>Enrique Sánchez</t>
+  </si>
+  <si>
+    <t>1965-02-05</t>
+  </si>
+  <si>
+    <t>Sporting Gijón</t>
+  </si>
+  <si>
+    <t>Joan Francesc Sicilia</t>
+  </si>
+  <si>
+    <t>1970-02-05</t>
+  </si>
+  <si>
+    <t>Ernesto Valverde</t>
+  </si>
+  <si>
+    <t>1964-02-09</t>
+  </si>
+  <si>
+    <t>Real Sociedad de Fútbol</t>
+  </si>
+  <si>
+    <t>Eusebio Sacristán</t>
+  </si>
+  <si>
+    <t>1964-04-13</t>
+  </si>
+  <si>
+    <t>Zinedine Zidane</t>
+  </si>
+  <si>
+    <t>1972-06-23</t>
+  </si>
+  <si>
+    <t>Diego Simeone</t>
+  </si>
+  <si>
+    <t>1970-04-28</t>
+  </si>
+  <si>
+    <t>Club Atlético de Madrid</t>
+  </si>
+  <si>
+    <t>Mauricio Pellegrino</t>
+  </si>
+  <si>
+    <t>Deportivo Alavés</t>
+  </si>
+  <si>
+    <t>1971-10-05</t>
+  </si>
+  <si>
+    <t>Eduardo Berizzoa</t>
+  </si>
+  <si>
+    <t>1969-11-13</t>
+  </si>
+  <si>
+    <t>Asier Garitano</t>
+  </si>
+  <si>
+    <t>1969-12-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salvador González </t>
+  </si>
+  <si>
+    <t>1963-10-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enrique Setién </t>
+  </si>
+  <si>
+    <t>1958-09-27</t>
+  </si>
+  <si>
+    <t>Urs Fischer</t>
+  </si>
+  <si>
+    <t>1966-02-20</t>
+  </si>
+  <si>
+    <t>Georgi Dermendzhiev</t>
+  </si>
+  <si>
+    <t>1955-01-04</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FC Bayern München </t>
+  </si>
+  <si>
+    <t>Carlo Ancelotti</t>
+  </si>
+  <si>
+    <t>1959-06-10</t>
+  </si>
+  <si>
+    <t>Ivan Daniliants</t>
+  </si>
+  <si>
+    <t>1953-02-20</t>
+  </si>
+  <si>
+    <t>USSR</t>
+  </si>
+  <si>
+    <t>Phillip Cocu</t>
+  </si>
+  <si>
+    <t>1970-10-29</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Brendan Rodgers</t>
+  </si>
+  <si>
+    <t>1973-01-26</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Serhiy Rebrov</t>
+  </si>
+  <si>
+    <t>1974-06-03</t>
+  </si>
+  <si>
+    <t>Soviet Union</t>
+  </si>
+  <si>
+    <t>Rui Vitória</t>
+  </si>
+  <si>
+    <t>1970-04-16</t>
+  </si>
+  <si>
+    <t>Şenol Güneş</t>
+  </si>
+  <si>
+    <t>1952-06-01</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Unai Emery</t>
+  </si>
+  <si>
+    <t>1971-11-03</t>
+  </si>
+  <si>
+    <t>Jacek Magiera</t>
+  </si>
+  <si>
+    <t>1977-01-01</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>1973-08-29</t>
+  </si>
+  <si>
+    <t>Thomas Tuchel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bruno Génésio</t>
+  </si>
+  <si>
+    <t>1966-09-01</t>
+  </si>
+  <si>
+    <t>Ivaylo Petev</t>
+  </si>
+  <si>
+    <t>1975-07-09</t>
+  </si>
+  <si>
+    <t>Nuno Espírito Santo</t>
+  </si>
+  <si>
+    <t>1974-01-25</t>
+  </si>
+  <si>
+    <t>Ståle Solbakken</t>
+  </si>
+  <si>
+    <t>1968-02-27</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Michel Preud'homme</t>
+  </si>
+  <si>
+    <t>1959-01-24</t>
+  </si>
+  <si>
+    <t>Belguim</t>
+  </si>
+  <si>
+    <t>Jorge Jesus</t>
+  </si>
+  <si>
+    <t>1954-07-24</t>
+  </si>
+  <si>
+    <t>Tayfun Korkut</t>
+  </si>
+  <si>
+    <t>1974-04-02</t>
+  </si>
+  <si>
+    <t>Viktar Hancharenka</t>
+  </si>
+  <si>
+    <t>1977-06-10</t>
+  </si>
+  <si>
+    <t>Bor. Mönchengladbach</t>
+  </si>
+  <si>
+    <t>Dieter Hecking</t>
+  </si>
+  <si>
+    <t>1964-09-12</t>
+  </si>
+  <si>
+    <t>Leonardo Jardim</t>
+  </si>
+  <si>
+    <t>1974-08-01</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Alexander Nouri</t>
+  </si>
+  <si>
+    <t>1979-08-20</t>
+  </si>
+  <si>
+    <t>Manuel Baum</t>
+  </si>
+  <si>
+    <t>1979-08-30</t>
+  </si>
+  <si>
+    <t>Andries Jonker</t>
+  </si>
+  <si>
+    <t>1962-09-22</t>
+  </si>
+  <si>
+    <t>Martin Schmidt</t>
+  </si>
+  <si>
+    <t>1967-04-12</t>
+  </si>
+  <si>
+    <t>Niko Kovač</t>
+  </si>
+  <si>
+    <t>1971-10-15</t>
+  </si>
+  <si>
+    <t>Markus Weinzierl</t>
+  </si>
+  <si>
+    <t>1974-12-28</t>
+  </si>
+  <si>
+    <t>Markus Gisdol</t>
+  </si>
+  <si>
+    <t>1969-08-17</t>
+  </si>
+  <si>
+    <t>Maik Walpurgis</t>
+  </si>
+  <si>
+    <t>1973-10-09</t>
+  </si>
+  <si>
+    <t>1. FC Köln</t>
+  </si>
+  <si>
+    <t>Peter Stöger</t>
+  </si>
+  <si>
+    <t>1966-04-11</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Torsten Frings</t>
+  </si>
+  <si>
+    <t>1976-11-22</t>
+  </si>
+  <si>
+    <t>Pál Dárdai</t>
+  </si>
+  <si>
+    <t>1976-03-16</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Christian Streich</t>
+  </si>
+  <si>
+    <t>1965-06-11</t>
+  </si>
+  <si>
+    <t>Julian Nagelsmann</t>
+  </si>
+  <si>
+    <t>1987-07-23</t>
+  </si>
+  <si>
+    <t>Ralph Hasenhüttl</t>
+  </si>
+  <si>
+    <t>1967-08-09</t>
   </si>
 </sst>
 </file>
@@ -908,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -917,816 +1319,1365 @@
     <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D9" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D10" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D12" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D13" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D16" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D18" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D19" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D20" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D21" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D23" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B24" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D24" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B25" t="s">
         <v>22</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D25" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B26" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D26" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D27" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B28" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D28" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B29" t="s">
         <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D29" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B30" t="s">
         <v>27</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D30" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B31" t="s">
         <v>28</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D31" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B32" t="s">
         <v>29</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D32" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B33" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D33" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B34" t="s">
         <v>31</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="D34" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B35" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="D35" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B36" t="s">
         <v>32</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D36" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>175</v>
+      </c>
       <c r="B37" t="s">
         <v>33</v>
       </c>
+      <c r="C37" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D37" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>177</v>
+      </c>
       <c r="B38" t="s">
         <v>34</v>
       </c>
+      <c r="C38" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D38" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>180</v>
+      </c>
       <c r="B39" t="s">
         <v>35</v>
       </c>
+      <c r="C39" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D39" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>182</v>
+      </c>
       <c r="B40" t="s">
         <v>36</v>
       </c>
+      <c r="C40" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D40" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>184</v>
+      </c>
       <c r="B41" t="s">
         <v>37</v>
       </c>
+      <c r="C41" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D41" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>186</v>
+      </c>
       <c r="B42" t="s">
+        <v>187</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D42" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>189</v>
+      </c>
+      <c r="B43" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
+      <c r="C43" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D43" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>191</v>
+      </c>
+      <c r="B44" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
+      <c r="C44" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D44" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>193</v>
+      </c>
+      <c r="B45" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
+      <c r="C45" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>195</v>
+      </c>
+      <c r="B46" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
+      <c r="C46" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D46" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>197</v>
+      </c>
+      <c r="B47" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
+      <c r="C47" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D47" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>199</v>
+      </c>
+      <c r="B48" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
+      <c r="C48" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D48" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>201</v>
+      </c>
+      <c r="B49" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
+      <c r="C49" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D49" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>203</v>
+      </c>
+      <c r="B50" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
+      <c r="C50" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D50" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>205</v>
+      </c>
+      <c r="B51" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
+      <c r="C51" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D51" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>208</v>
+      </c>
+      <c r="B52" t="s">
+        <v>207</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>210</v>
+      </c>
+      <c r="B53" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
+      <c r="C53" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D53" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>213</v>
+      </c>
+      <c r="B54" t="s">
+        <v>212</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D54" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>215</v>
+      </c>
+      <c r="B55" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
+      <c r="C55" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D55" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>217</v>
+      </c>
+      <c r="B56" t="s">
+        <v>219</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D56" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>220</v>
+      </c>
+      <c r="B57" t="s">
+        <v>221</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D57" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>223</v>
+      </c>
+      <c r="B58" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
+      <c r="C58" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D58" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>225</v>
+      </c>
+      <c r="B59" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
+      <c r="C59" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>227</v>
+      </c>
+      <c r="B60" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
+      <c r="C60" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D60" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>229</v>
+      </c>
+      <c r="B61" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
+      <c r="C61" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>231</v>
+      </c>
+      <c r="B62" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
+      <c r="C62" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D62" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>233</v>
+      </c>
+      <c r="B63" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
+      <c r="C63" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D63" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>237</v>
+      </c>
+      <c r="B64" t="s">
+        <v>236</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D64" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>239</v>
+      </c>
+      <c r="B65" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B60" t="s">
+      <c r="C65" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D65" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>242</v>
+      </c>
+      <c r="B66" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
+      <c r="C66" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D66" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>245</v>
+      </c>
+      <c r="B67" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
+      <c r="C67" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D67" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>248</v>
+      </c>
+      <c r="B68" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B63" t="s">
+      <c r="C68" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D68" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>251</v>
+      </c>
+      <c r="B69" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
+      <c r="C69" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D69" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>253</v>
+      </c>
+      <c r="B70" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
+      <c r="C70" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D70" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>256</v>
+      </c>
+      <c r="B71" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B66" t="s">
+      <c r="C71" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D71" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>258</v>
+      </c>
+      <c r="B72" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
+      <c r="C72" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D72" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>262</v>
+      </c>
+      <c r="B73" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
+      <c r="C73" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D73" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>263</v>
+      </c>
+      <c r="B74" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B69" t="s">
+      <c r="C74" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D74" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>265</v>
+      </c>
+      <c r="B75" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B70" t="s">
+      <c r="C75" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D75" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>267</v>
+      </c>
+      <c r="B76" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B71" t="s">
+      <c r="C76" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D76" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>269</v>
+      </c>
+      <c r="B77" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B72" t="s">
+      <c r="C77" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D77" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>272</v>
+      </c>
+      <c r="B78" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B73" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B74" t="s">
+      <c r="C78" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D78" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>275</v>
+      </c>
+      <c r="B79" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B75" t="s">
+      <c r="C79" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D79" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>277</v>
+      </c>
+      <c r="B80" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B76" t="s">
+      <c r="C80" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D80" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>279</v>
+      </c>
+      <c r="B81" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B77" t="s">
+      <c r="C81" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D81" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>282</v>
+      </c>
+      <c r="B82" t="s">
+        <v>281</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D82" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>284</v>
+      </c>
+      <c r="B83" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B78" t="s">
+      <c r="C83" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D83" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>287</v>
+      </c>
+      <c r="B84" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B79" t="s">
+      <c r="C84" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D84" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>289</v>
+      </c>
+      <c r="B85" t="s">
+        <v>75</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D85" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>291</v>
+      </c>
+      <c r="B86" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B80" t="s">
+      <c r="C86" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D86" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>293</v>
+      </c>
+      <c r="B87" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B81" t="s">
+      <c r="C87" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D87" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>295</v>
+      </c>
+      <c r="B88" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B82" t="s">
+      <c r="C88" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D88" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>297</v>
+      </c>
+      <c r="B89" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B83" t="s">
+      <c r="C89" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D89" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>299</v>
+      </c>
+      <c r="B90" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B84" t="s">
+      <c r="C90" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D90" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>301</v>
+      </c>
+      <c r="B91" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B85" t="s">
+      <c r="C91" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D91" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>304</v>
+      </c>
+      <c r="B92" t="s">
+        <v>303</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D92" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>307</v>
+      </c>
+      <c r="B93" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B86" t="s">
+      <c r="C93" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D93" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>309</v>
+      </c>
+      <c r="B94" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B87" t="s">
+      <c r="C94" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D94" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>312</v>
+      </c>
+      <c r="B95" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B88" t="s">
+      <c r="C95" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D95" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>314</v>
+      </c>
+      <c r="B96" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B89" t="s">
+      <c r="C96" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D96" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>316</v>
+      </c>
+      <c r="B97" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B90" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B91" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B92" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B93" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B94" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B95" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B96" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B97" t="s">
-        <v>94</v>
+      <c r="C97" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D97" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>